<commit_message>
got secondi solving to work!
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinnguyen\Documents\Code\Projects\bomboniera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47F3F12-01C7-490B-869D-2ECA84FBFAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C083EA-411D-4389-A937-AD55E9D3AB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" firstSheet="2" activeTab="4" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
   </bookViews>
   <sheets>
     <sheet name="capacity_female" sheetId="4" r:id="rId1"/>
     <sheet name="capacity_male" sheetId="1" r:id="rId2"/>
     <sheet name="choices_female" sheetId="2" r:id="rId3"/>
     <sheet name="choices_male" sheetId="5" r:id="rId4"/>
+    <sheet name="culturalgroup_male" sheetId="7" r:id="rId5"/>
+    <sheet name="culturalgroup_female" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="109">
   <si>
     <t>student</t>
   </si>
@@ -343,13 +345,34 @@
   </si>
   <si>
     <t>AI</t>
+  </si>
+  <si>
+    <t>cultural group</t>
+  </si>
+  <si>
+    <t>ASIA</t>
+  </si>
+  <si>
+    <t>ESEU</t>
+  </si>
+  <si>
+    <t>MENA</t>
+  </si>
+  <si>
+    <t>ITAL</t>
+  </si>
+  <si>
+    <t>ALTR</t>
+  </si>
+  <si>
+    <t>LTIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +385,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="BitstromWera Nerd Font"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -384,8 +413,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2654,8 +2684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932AD7BC-7322-48CC-B1D8-642C08DDB1CE}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,7 +4379,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5079,4 +5109,851 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC41016-7674-45F3-A248-481CDEA79CE2}">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB8A3BD-5C93-4091-BA66-2BB59C536437}">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented coupling (or toupling) but not sure if it is unbiased completely
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinnguyen\Documents\Code\Projects\bomboniera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C083EA-411D-4389-A937-AD55E9D3AB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1786BED-063D-4CD8-9EBE-B7F5E656F732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" firstSheet="2" activeTab="4" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
   </bookViews>
   <sheets>
     <sheet name="capacity_female" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="111">
   <si>
     <t>student</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>LTIN</t>
+  </si>
+  <si>
+    <t>tuple</t>
+  </si>
+  <si>
+    <t>A and B</t>
   </si>
 </sst>
 </file>
@@ -2874,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E88CA73-73FE-47D8-BDE1-A388110E1A5F}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,7 +2891,7 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2910,8 +2916,11 @@
       <c r="H1">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2936,8 +2945,11 @@
       <c r="H2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2962,8 +2974,11 @@
       <c r="H3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2988,8 +3003,11 @@
       <c r="H4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3014,8 +3032,11 @@
       <c r="H5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3040,8 +3061,11 @@
       <c r="H6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3066,8 +3090,11 @@
       <c r="H7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3092,8 +3119,11 @@
       <c r="H8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3118,8 +3148,11 @@
       <c r="H9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -3144,8 +3177,11 @@
       <c r="H10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -3170,8 +3206,11 @@
       <c r="H11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3196,8 +3235,11 @@
       <c r="H12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3222,8 +3264,11 @@
       <c r="H13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3248,8 +3293,11 @@
       <c r="H14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3274,8 +3322,11 @@
       <c r="H15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3300,8 +3351,11 @@
       <c r="H16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3326,8 +3380,11 @@
       <c r="H17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3352,8 +3409,11 @@
       <c r="H18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3378,8 +3438,11 @@
       <c r="H19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3404,8 +3467,11 @@
       <c r="H20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3430,8 +3496,11 @@
       <c r="H21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3456,8 +3525,11 @@
       <c r="H22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3482,8 +3554,11 @@
       <c r="H23" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3508,8 +3583,11 @@
       <c r="H24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3534,8 +3612,11 @@
       <c r="H25" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3560,8 +3641,11 @@
       <c r="H26" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3586,8 +3670,11 @@
       <c r="H27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3612,8 +3699,11 @@
       <c r="H28" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3638,8 +3728,11 @@
       <c r="H29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3664,8 +3757,11 @@
       <c r="H30" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3690,8 +3786,11 @@
       <c r="H31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3716,8 +3815,11 @@
       <c r="H32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -3742,8 +3844,11 @@
       <c r="H33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -3768,8 +3873,11 @@
       <c r="H34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3794,8 +3902,11 @@
       <c r="H35" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3820,8 +3931,11 @@
       <c r="H36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3846,8 +3960,11 @@
       <c r="H37" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3872,8 +3989,11 @@
       <c r="H38" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3898,8 +4018,11 @@
       <c r="H39" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3924,8 +4047,11 @@
       <c r="H40" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3950,8 +4076,11 @@
       <c r="H41" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3976,8 +4105,11 @@
       <c r="H42" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -4002,8 +4134,11 @@
       <c r="H43" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -4028,8 +4163,11 @@
       <c r="H44" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -4054,8 +4192,11 @@
       <c r="H45" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -4080,8 +4221,11 @@
       <c r="H46" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -4106,8 +4250,11 @@
       <c r="H47" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -4132,8 +4279,11 @@
       <c r="H48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -4158,8 +4308,11 @@
       <c r="H49" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -4184,8 +4337,11 @@
       <c r="H50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -4210,8 +4366,11 @@
       <c r="H51" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -4236,8 +4395,11 @@
       <c r="H52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -4262,8 +4424,11 @@
       <c r="H53" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -4288,8 +4453,11 @@
       <c r="H54" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -4314,8 +4482,11 @@
       <c r="H55" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -4340,8 +4511,11 @@
       <c r="H56" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -4365,6 +4539,9 @@
       </c>
       <c r="H57" t="s">
         <v>63</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4376,15 +4553,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB8F0D-C323-4725-8B27-EB6989D943B6}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4403,10 +4580,13 @@
       <c r="F1">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -4423,70 +4603,82 @@
       <c r="F2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -4503,10 +4695,13 @@
       <c r="F6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -4515,18 +4710,21 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
@@ -4543,10 +4741,13 @@
       <c r="F8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -4563,90 +4764,105 @@
       <c r="F9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>60</v>
@@ -4658,41 +4874,47 @@
         <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
@@ -4703,19 +4925,22 @@
       <c r="F16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
         <v>66</v>
@@ -4723,19 +4948,22 @@
       <c r="F17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
         <v>66</v>
@@ -4743,10 +4971,13 @@
       <c r="F18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
@@ -4758,35 +4989,41 @@
         <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
         <v>60</v>
@@ -4803,10 +5040,13 @@
       <c r="F21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
@@ -4815,18 +5055,21 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
         <v>60</v>
@@ -4835,18 +5078,21 @@
         <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -4855,18 +5101,21 @@
         <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
         <v>60</v>
@@ -4875,18 +5124,21 @@
         <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -4895,18 +5147,21 @@
         <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
         <v>60</v>
@@ -4915,18 +5170,21 @@
         <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -4943,50 +5201,59 @@
       <c r="F28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
         <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
         <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
@@ -5003,10 +5270,13 @@
       <c r="F31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
@@ -5023,10 +5293,13 @@
       <c r="F32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
         <v>60</v>
@@ -5035,18 +5308,21 @@
         <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
         <v>60</v>
@@ -5055,18 +5331,21 @@
         <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F34" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
         <v>60</v>
@@ -5075,33 +5354,16 @@
         <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" t="s">
-        <v>66</v>
+      <c r="G35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5115,7 +5377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC41016-7674-45F3-A248-481CDEA79CE2}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished solver and added export to xlsx
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinnguyen\Documents\Code\Projects\bomboniera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B881FFF-A080-4B9E-BBC8-AB3E4217B581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56649AFD-A54F-4263-A887-3D057BA0C955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{1558DEF6-6C37-4150-9CCF-8C8D530D7643}"/>
   </bookViews>
   <sheets>
     <sheet name="capacity_female" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="144">
   <si>
     <t>student</t>
   </si>
@@ -714,7 +714,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -2790,8 +2790,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,7 +2840,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4829,7 +4829,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -5763,8 +5763,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33:J57"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7565,36 +7565,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" t="s">
-        <v>61</v>
-      </c>
-      <c r="F57" t="s">
-        <v>62</v>
-      </c>
-      <c r="G57" t="s">
-        <v>66</v>
-      </c>
-      <c r="H57" t="s">
-        <v>63</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="J57" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>